<commit_message>
Fixed Programs cost and coverage calc formulas
</commit_message>
<xml_diff>
--- a/inputs/demo_region2_input.xlsx
+++ b/inputs/demo_region2_input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\regional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21144" windowWidth="38400" windowHeight="21144" tabRatio="961" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4814,14 +4814,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="14.44140625" style="12"/>
+    <col min="1" max="1" width="27.6328125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6328125" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="14.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4832,14 +4832,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>193</v>
@@ -4848,7 +4848,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>192</v>
@@ -4857,7 +4857,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -4926,7 +4926,7 @@
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
         <v>129</v>
       </c>
@@ -5067,7 +5067,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -5271,13 +5271,13 @@
       <selection activeCell="C2" sqref="C2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="55" customWidth="1"/>
-    <col min="2" max="16384" width="10.77734375" style="55"/>
+    <col min="1" max="1" width="18.6328125" style="55" customWidth="1"/>
+    <col min="2" max="16384" width="10.81640625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>195</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
         <v>164</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="57"/>
       <c r="B3" s="57" t="s">
         <v>1</v>
@@ -5329,7 +5329,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="57"/>
       <c r="B4" s="57" t="s">
         <v>2</v>
@@ -5346,7 +5346,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="57"/>
       <c r="B5" s="57" t="s">
         <v>3</v>
@@ -5363,7 +5363,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="57"/>
       <c r="B6" s="57" t="s">
         <v>4</v>
@@ -5380,7 +5380,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" s="56"/>
     </row>
   </sheetData>
@@ -5400,15 +5400,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="35"/>
+    <col min="2" max="2" width="47.81640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
         <v>187</v>
       </c>
@@ -5428,7 +5428,7 @@
       </c>
       <c r="C2" s="84"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
         <v>209</v>
       </c>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="C3" s="84"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
         <v>58</v>
       </c>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="C4" s="84"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>137</v>
       </c>
@@ -5455,77 +5455,77 @@
       </c>
       <c r="C5" s="84"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
       <c r="B6" s="90"/>
       <c r="C6" s="90"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="90"/>
       <c r="C9" s="90"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="91"/>
       <c r="B11" s="90"/>
       <c r="C11" s="90"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="91"/>
       <c r="B12" s="90"/>
       <c r="C12" s="90"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="91"/>
       <c r="B13" s="90"/>
       <c r="C13" s="90"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="91"/>
       <c r="B14" s="90"/>
       <c r="C14" s="90"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="91"/>
       <c r="B15" s="90"/>
       <c r="C15" s="90"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="91"/>
       <c r="B16" s="90"/>
       <c r="C16" s="90"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="90"/>
       <c r="C17" s="90"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="90"/>
       <c r="C18" s="90"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="89"/>
       <c r="B19" s="90"/>
       <c r="C19" s="90"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="89"/>
       <c r="B20" s="90"/>
       <c r="C20" s="90"/>
@@ -5549,85 +5549,85 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="35"/>
+    <col min="1" max="1" width="30.08984375" style="35" customWidth="1"/>
+    <col min="2" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="48"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
     </row>
   </sheetData>
@@ -5647,7 +5647,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -5757,23 +5757,23 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="C29" activeCellId="3" sqref="C2:O12 C14:O21 C23:O27 C29:O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -6335,7 +6335,7 @@
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>86</v>
@@ -6431,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>187</v>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>209</v>
@@ -6716,7 +6716,7 @@
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="62" t="s">
         <v>37</v>
       </c>
@@ -6966,7 +6966,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -7475,7 +7475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
@@ -7513,16 +7513,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="35" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" style="35"/>
-    <col min="5" max="5" width="17.44140625" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="35"/>
+    <col min="1" max="1" width="33.6328125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" style="35"/>
+    <col min="5" max="5" width="17.453125" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>163</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>157</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>156</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>155</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>153</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>152</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>151</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>150</v>
       </c>
@@ -7722,20 +7722,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.90625" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" style="57" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="57" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.33203125" style="57" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.88671875" style="57" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="16.109375" style="57"/>
+    <col min="6" max="7" width="13.08984375" style="57" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.36328125" style="57" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.90625" style="57" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.08984375" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
         <v>33</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="59" t="s">
         <v>31</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="52" t="s">
         <v>149</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="52" t="s">
         <v>173</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="52" t="s">
         <v>199</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="52" t="s">
         <v>200</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="52" t="s">
         <v>196</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="52" t="s">
         <v>136</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="52" t="s">
         <v>137</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="52" t="s">
         <v>84</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="52" t="s">
         <v>58</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="52" t="s">
         <v>67</v>
       </c>
@@ -8269,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="52" t="s">
         <v>28</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="52" t="s">
         <v>85</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="52" t="s">
         <v>60</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="52"/>
       <c r="C16" s="96"/>
       <c r="D16" s="96"/>
@@ -8417,7 +8417,7 @@
       <c r="N16" s="96"/>
       <c r="O16" s="96"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
         <v>32</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="59"/>
       <c r="B18" s="52" t="s">
         <v>86</v>
@@ -8509,7 +8509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="97" t="s">
         <v>187</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="97" t="s">
         <v>209</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="98" t="s">
         <v>57</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="52" t="s">
         <v>88</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="52" t="s">
         <v>87</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="52" t="s">
         <v>59</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="52"/>
       <c r="C25" s="96"/>
       <c r="D25" s="96"/>
@@ -8789,7 +8789,7 @@
       <c r="N25" s="96"/>
       <c r="O25" s="96"/>
     </row>
-    <row r="26" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="59" t="s">
         <v>37</v>
       </c>
@@ -8837,7 +8837,7 @@
       </c>
       <c r="P26" s="99"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="63" t="s">
         <v>188</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="59"/>
       <c r="B28" s="63" t="s">
         <v>208</v>
@@ -8926,7 +8926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="63" t="s">
         <v>189</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="63" t="s">
         <v>190</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="52"/>
       <c r="C31" s="100"/>
       <c r="D31" s="100"/>
@@ -9030,7 +9030,7 @@
       <c r="N31" s="96"/>
       <c r="O31" s="96"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="59" t="s">
         <v>35</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="52" t="s">
         <v>64</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="52" t="s">
         <v>62</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="52" t="s">
         <v>47</v>
       </c>
@@ -9209,7 +9209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="52" t="s">
         <v>34</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="102"/>
       <c r="B37" s="52" t="s">
         <v>83</v>
@@ -9298,7 +9298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="52" t="s">
         <v>82</v>
       </c>
@@ -9342,7 +9342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="52" t="s">
         <v>81</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" s="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="52" t="s">
         <v>79</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="52" t="s">
         <v>80</v>
       </c>
@@ -9491,22 +9491,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="58.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="J2" s="95"/>
       <c r="K2" s="95"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>86</v>
       </c>
@@ -9575,7 +9575,7 @@
       <c r="J3" s="95"/>
       <c r="K3" s="95"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>61</v>
       </c>
@@ -9592,7 +9592,7 @@
       <c r="J4" s="95"/>
       <c r="K4" s="95"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>149</v>
       </c>
@@ -9609,7 +9609,7 @@
       <c r="J5" s="95"/>
       <c r="K5" s="95"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>198</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>63</v>
       </c>
@@ -9647,7 +9647,7 @@
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>64</v>
       </c>
@@ -9666,7 +9666,7 @@
       <c r="J8" s="95"/>
       <c r="K8" s="95"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>62</v>
       </c>
@@ -9685,7 +9685,7 @@
       <c r="J9" s="95"/>
       <c r="K9" s="95"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>188</v>
       </c>
@@ -9702,7 +9702,7 @@
       <c r="J10" s="95"/>
       <c r="K10" s="95"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
         <v>208</v>
       </c>
@@ -9719,7 +9719,7 @@
       <c r="J11" s="95"/>
       <c r="K11" s="95"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>189</v>
       </c>
@@ -9736,7 +9736,7 @@
       <c r="J12" s="95"/>
       <c r="K12" s="95"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>190</v>
       </c>
@@ -9753,7 +9753,7 @@
       <c r="J13" s="95"/>
       <c r="K13" s="95"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="97" t="s">
         <v>187</v>
       </c>
@@ -9772,7 +9772,7 @@
       <c r="J14" s="95"/>
       <c r="K14" s="95"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="97" t="s">
         <v>209</v>
       </c>
@@ -9791,7 +9791,7 @@
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>57</v>
       </c>
@@ -9812,7 +9812,7 @@
       <c r="J16" s="95"/>
       <c r="K16" s="95"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>47</v>
       </c>
@@ -9829,7 +9829,7 @@
       <c r="J17" s="95"/>
       <c r="K17" s="95"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>173</v>
       </c>
@@ -9848,7 +9848,7 @@
       <c r="J18" s="95"/>
       <c r="K18" s="95"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>199</v>
       </c>
@@ -9867,7 +9867,7 @@
       <c r="J19" s="95"/>
       <c r="K19" s="95"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
         <v>200</v>
       </c>
@@ -9886,7 +9886,7 @@
       <c r="J20" s="95"/>
       <c r="K20" s="95"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>196</v>
       </c>
@@ -9905,7 +9905,7 @@
       <c r="J21" s="95"/>
       <c r="K21" s="95"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
         <v>136</v>
       </c>
@@ -9926,7 +9926,7 @@
       <c r="J22" s="95"/>
       <c r="K22" s="95"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>34</v>
       </c>
@@ -9945,7 +9945,7 @@
       <c r="J23" s="95"/>
       <c r="K23" s="95"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="52" t="s">
         <v>88</v>
       </c>
@@ -9962,7 +9962,7 @@
       <c r="J24" s="95"/>
       <c r="K24" s="95"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
         <v>87</v>
       </c>
@@ -9979,7 +9979,7 @@
       <c r="J25" s="95"/>
       <c r="K25" s="95"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>137</v>
       </c>
@@ -9996,7 +9996,7 @@
       <c r="J26" s="95"/>
       <c r="K26" s="95"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>59</v>
       </c>
@@ -10015,7 +10015,7 @@
       <c r="J27" s="95"/>
       <c r="K27" s="95"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>84</v>
       </c>
@@ -10032,7 +10032,7 @@
       <c r="J28" s="95"/>
       <c r="K28" s="95"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>58</v>
       </c>
@@ -10051,7 +10051,7 @@
       <c r="J29" s="95"/>
       <c r="K29" s="95"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
         <v>67</v>
       </c>
@@ -10068,7 +10068,7 @@
       <c r="J30" s="95"/>
       <c r="K30" s="95"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
         <v>28</v>
       </c>
@@ -10087,7 +10087,7 @@
       <c r="J31" s="95"/>
       <c r="K31" s="95"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>83</v>
       </c>
@@ -10106,7 +10106,7 @@
       <c r="J32" s="95"/>
       <c r="K32" s="95"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
         <v>82</v>
       </c>
@@ -10125,7 +10125,7 @@
       <c r="J33" s="95"/>
       <c r="K33" s="95"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>81</v>
       </c>
@@ -10144,7 +10144,7 @@
       <c r="J34" s="95"/>
       <c r="K34" s="95"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>79</v>
       </c>
@@ -10163,7 +10163,7 @@
       <c r="J35" s="95"/>
       <c r="K35" s="95"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A36" s="52" t="s">
         <v>80</v>
       </c>
@@ -10182,7 +10182,7 @@
       <c r="J36" s="95"/>
       <c r="K36" s="95"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
         <v>85</v>
       </c>
@@ -10199,7 +10199,7 @@
       <c r="J37" s="95"/>
       <c r="K37" s="95"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>60</v>
       </c>
@@ -10237,22 +10237,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="16.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>218</v>
       </c>
@@ -10287,7 +10287,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -10316,7 +10316,7 @@
       <c r="J2" s="95"/>
       <c r="K2" s="95"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -10345,7 +10345,7 @@
       <c r="J3" s="95"/>
       <c r="K3" s="95"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -10374,7 +10374,7 @@
       <c r="J4" s="95"/>
       <c r="K4" s="95"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
@@ -10403,7 +10403,7 @@
       <c r="J5" s="95"/>
       <c r="K5" s="95"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
@@ -10432,7 +10432,7 @@
       <c r="J6" s="95"/>
       <c r="K6" s="95"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>53</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>54</v>
       </c>
@@ -10474,7 +10474,7 @@
       <c r="J8" s="95"/>
       <c r="K8" s="95"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>55</v>
       </c>
@@ -10495,7 +10495,7 @@
       <c r="J9" s="95"/>
       <c r="K9" s="95"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
@@ -10516,7 +10516,7 @@
       <c r="J10" s="95"/>
       <c r="K10" s="95"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>49</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>50</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>51</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>52</v>
       </c>
@@ -10611,14 +10611,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="12" customWidth="1"/>
-    <col min="2" max="9" width="16.77734375" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="14.44140625" style="12"/>
+    <col min="1" max="1" width="8.453125" style="12" customWidth="1"/>
+    <col min="2" max="9" width="16.81640625" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="14.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -11707,15 +11707,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="48.08984375" style="35" customWidth="1"/>
     <col min="2" max="2" width="15" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="12.77734375" style="35"/>
+    <col min="3" max="3" width="14.6328125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>219</v>
       </c>
@@ -11741,7 +11741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>220</v>
       </c>
@@ -11767,7 +11767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="142"/>
       <c r="C3" s="35" t="s">
         <v>175</v>
@@ -11789,7 +11789,7 @@
       </c>
       <c r="J3" s="105"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B4" s="142"/>
       <c r="C4" s="35" t="s">
         <v>174</v>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="J4" s="105"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="142" t="s">
         <v>1</v>
       </c>
@@ -11835,7 +11835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B6" s="142"/>
       <c r="C6" s="35" t="s">
         <v>175</v>
@@ -11856,7 +11856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B7" s="142"/>
       <c r="C7" s="35" t="s">
         <v>174</v>
@@ -11877,7 +11877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B8" s="142" t="s">
         <v>2</v>
       </c>
@@ -11900,7 +11900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B9" s="142"/>
       <c r="C9" s="35" t="s">
         <v>175</v>
@@ -11921,7 +11921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B10" s="142"/>
       <c r="C10" s="35" t="s">
         <v>174</v>
@@ -11942,7 +11942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="142" t="s">
         <v>3</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B12" s="142"/>
       <c r="C12" s="35" t="s">
         <v>175</v>
@@ -11986,7 +11986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B13" s="142"/>
       <c r="C13" s="35" t="s">
         <v>174</v>
@@ -12007,7 +12007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B14" s="142" t="s">
         <v>4</v>
       </c>
@@ -12030,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B15" s="142"/>
       <c r="C15" s="35" t="s">
         <v>175</v>
@@ -12051,7 +12051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B16" s="142"/>
       <c r="C16" s="35" t="s">
         <v>174</v>
@@ -12072,7 +12072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B17" s="106" t="s">
         <v>172</v>
       </c>
@@ -12095,14 +12095,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="D18" s="107"/>
       <c r="E18" s="107"/>
       <c r="F18" s="107"/>
       <c r="G18" s="107"/>
       <c r="H18" s="107"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>221</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B20" s="142"/>
       <c r="C20" s="35" t="s">
         <v>175</v>
@@ -12149,7 +12149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B21" s="142"/>
       <c r="C21" s="35" t="s">
         <v>174</v>
@@ -12170,7 +12170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B22" s="142" t="s">
         <v>1</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B23" s="142"/>
       <c r="C23" s="35" t="s">
         <v>175</v>
@@ -12214,7 +12214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B24" s="142"/>
       <c r="C24" s="35" t="s">
         <v>174</v>
@@ -12235,7 +12235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B25" s="142" t="s">
         <v>2</v>
       </c>
@@ -12258,7 +12258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B26" s="142"/>
       <c r="C26" s="35" t="s">
         <v>175</v>
@@ -12279,7 +12279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B27" s="142"/>
       <c r="C27" s="35" t="s">
         <v>174</v>
@@ -12300,7 +12300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B28" s="142" t="s">
         <v>3</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B29" s="142"/>
       <c r="C29" s="35" t="s">
         <v>175</v>
@@ -12344,7 +12344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B30" s="142"/>
       <c r="C30" s="35" t="s">
         <v>174</v>
@@ -12365,7 +12365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B31" s="142" t="s">
         <v>4</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B32" s="142"/>
       <c r="C32" s="35" t="s">
         <v>175</v>
@@ -12409,7 +12409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B33" s="142"/>
       <c r="C33" s="35" t="s">
         <v>174</v>
@@ -12430,7 +12430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B34" s="106" t="s">
         <v>172</v>
       </c>
@@ -12453,14 +12453,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="D35" s="107"/>
       <c r="E35" s="107"/>
       <c r="F35" s="107"/>
       <c r="G35" s="107"/>
       <c r="H35" s="107"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="108" t="s">
         <v>222</v>
       </c>
@@ -12486,7 +12486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B37" s="142"/>
       <c r="C37" s="35" t="s">
         <v>175</v>
@@ -12507,7 +12507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B38" s="142"/>
       <c r="C38" s="35" t="s">
         <v>174</v>
@@ -12528,7 +12528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B39" s="142" t="s">
         <v>1</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B40" s="142"/>
       <c r="C40" s="35" t="s">
         <v>175</v>
@@ -12572,7 +12572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B41" s="142"/>
       <c r="C41" s="35" t="s">
         <v>174</v>
@@ -12593,7 +12593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B42" s="142" t="s">
         <v>2</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B43" s="142"/>
       <c r="C43" s="35" t="s">
         <v>175</v>
@@ -12637,7 +12637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B44" s="142"/>
       <c r="C44" s="35" t="s">
         <v>174</v>
@@ -12658,7 +12658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B45" s="142" t="s">
         <v>3</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B46" s="142"/>
       <c r="C46" s="35" t="s">
         <v>175</v>
@@ -12702,7 +12702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B47" s="142"/>
       <c r="C47" s="35" t="s">
         <v>174</v>
@@ -12723,7 +12723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B48" s="142" t="s">
         <v>4</v>
       </c>
@@ -12746,7 +12746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B49" s="142"/>
       <c r="C49" s="35" t="s">
         <v>175</v>
@@ -12767,7 +12767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B50" s="142"/>
       <c r="C50" s="35" t="s">
         <v>174</v>
@@ -12788,7 +12788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="13" x14ac:dyDescent="0.25">
       <c r="B51" s="109" t="s">
         <v>172</v>
       </c>
@@ -12814,12 +12814,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12829,6 +12823,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12846,22 +12846,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="34.08984375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="35" customWidth="1"/>
     <col min="5" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="16.109375" style="35"/>
+    <col min="7" max="16384" width="16.08984375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="111" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="111" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="110" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="112"/>
       <c r="C2" s="113" t="s">
         <v>26</v>
@@ -12876,7 +12876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>224</v>
       </c>
@@ -12960,7 +12960,7 @@
       <c r="E8" s="105"/>
       <c r="F8" s="105"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
         <v>225</v>
       </c>
@@ -12985,7 +12985,7 @@
       <c r="F10" s="105"/>
       <c r="G10" s="122"/>
     </row>
-    <row r="11" spans="1:7" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="110" t="s">
         <v>226</v>
       </c>
@@ -12995,7 +12995,7 @@
       <c r="F11" s="124"/>
       <c r="G11" s="125"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
         <v>227</v>
       </c>
@@ -13059,7 +13059,7 @@
       </c>
       <c r="G15" s="122"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="40"/>
       <c r="B16" s="126"/>
       <c r="C16" s="127"/>
@@ -13068,7 +13068,7 @@
       <c r="F16" s="105"/>
       <c r="G16" s="122"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
         <v>231</v>
       </c>
@@ -13222,7 +13222,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="126"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="40"/>
     </row>
   </sheetData>
@@ -13243,23 +13243,23 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.21875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="35" customWidth="1"/>
-    <col min="4" max="8" width="14.77734375" style="35" customWidth="1"/>
-    <col min="9" max="12" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="27.1796875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" style="35" customWidth="1"/>
+    <col min="4" max="8" width="14.81640625" style="35" customWidth="1"/>
+    <col min="9" max="12" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="16.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="111" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="111" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="110" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="131" t="s">
         <v>213</v>
       </c>
@@ -13293,7 +13293,7 @@
       <c r="O2" s="133"/>
       <c r="P2" s="133"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="35" t="s">
         <v>71</v>
@@ -13726,7 +13726,7 @@
       <c r="O17" s="131"/>
       <c r="P17" s="131"/>
     </row>
-    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="43" t="s">
         <v>238</v>
       </c>
@@ -13984,12 +13984,12 @@
       <c r="O26" s="131"/>
       <c r="P26" s="131"/>
     </row>
-    <row r="28" spans="1:16" s="111" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="111" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="110" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="134" t="s">
         <v>240</v>
       </c>
@@ -14023,7 +14023,7 @@
       <c r="O29" s="133"/>
       <c r="P29" s="133"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="35" t="s">
         <v>71</v>
@@ -14718,12 +14718,12 @@
       <c r="C54" s="43"/>
       <c r="D54" s="43"/>
     </row>
-    <row r="55" spans="1:16" s="111" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="111" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="110" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A56" s="134" t="s">
         <v>70</v>
       </c>
@@ -14751,7 +14751,7 @@
       <c r="O56" s="133"/>
       <c r="P56" s="133"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="35" t="s">
         <v>38</v>
@@ -14897,12 +14897,12 @@
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
     </row>
-    <row r="64" spans="1:16" s="111" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="111" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="110" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A65" s="134" t="s">
         <v>24</v>
       </c>
@@ -14936,7 +14936,7 @@
       <c r="O65" s="133"/>
       <c r="P65" s="133"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="138"/>
       <c r="B66" s="35" t="s">
         <v>73</v>
@@ -15972,12 +15972,12 @@
       <c r="O101" s="131"/>
       <c r="P101" s="131"/>
     </row>
-    <row r="103" spans="1:16" s="111" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" s="111" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A103" s="110" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A104" s="134" t="s">
         <v>71</v>
       </c>
@@ -16011,7 +16011,7 @@
       <c r="O104" s="133"/>
       <c r="P104" s="133"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="36"/>
       <c r="C105" s="43" t="s">
@@ -16125,7 +16125,7 @@
       <c r="O108" s="131"/>
       <c r="P108" s="131"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
     </row>
   </sheetData>
@@ -16146,24 +16146,24 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="44.44140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="35" customWidth="1"/>
     <col min="6" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="7" max="7" width="13.6328125" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="110" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
         <v>25</v>
       </c>
@@ -16204,7 +16204,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="130" t="s">
         <v>252</v>
@@ -16225,7 +16225,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="115" t="s">
         <v>253</v>
       </c>
@@ -16298,12 +16298,12 @@
       <c r="F9" s="130"/>
       <c r="G9" s="130"/>
     </row>
-    <row r="10" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="110" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="115"/>
       <c r="B11" s="126" t="s">
         <v>196</v>
@@ -16324,16 +16324,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="115"/>
       <c r="B12" s="126"/>
     </row>
-    <row r="13" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="110" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="138" t="s">
         <v>240</v>
       </c>
@@ -16356,7 +16356,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="130" t="s">
         <v>257</v>
@@ -16377,7 +16377,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="138" t="s">
         <v>70</v>
       </c>
@@ -16401,12 +16401,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="111" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="110" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="115" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="115" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="59" t="s">
         <v>49</v>
       </c>
@@ -16456,16 +16456,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.21875" style="35" customWidth="1"/>
-    <col min="2" max="6" width="16.109375" style="35"/>
-    <col min="7" max="7" width="17.21875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="16.109375" style="35"/>
+    <col min="1" max="1" width="52.1796875" style="35" customWidth="1"/>
+    <col min="2" max="6" width="16.08984375" style="35"/>
+    <col min="7" max="7" width="17.1796875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="16.08984375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="132" t="s">
         <v>69</v>
       </c>
@@ -16735,15 +16735,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="58.90625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="15" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="12.77734375" style="35"/>
+    <col min="16" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="114" t="s">
@@ -16786,7 +16786,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>262</v>
       </c>
@@ -17231,7 +17231,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="63" t="s">
         <v>137</v>
       </c>
@@ -17319,7 +17319,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>263</v>
       </c>
@@ -17531,15 +17531,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" style="35" customWidth="1"/>
-    <col min="3" max="7" width="15.5546875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="1" max="1" width="21.36328125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="35" customWidth="1"/>
+    <col min="3" max="7" width="15.54296875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40"/>
       <c r="B1" s="132"/>
       <c r="C1" s="40" t="s">
@@ -17558,12 +17558,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="63" t="s">
         <v>67</v>
       </c>
@@ -17583,7 +17583,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>265</v>
       </c>
@@ -17594,7 +17594,7 @@
       <c r="F4" s="140"/>
       <c r="G4" s="140"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="97" t="s">
         <v>183</v>
       </c>
@@ -17632,20 +17632,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" style="52" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" style="52" customWidth="1"/>
     <col min="4" max="4" width="15" style="35" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="35" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="35"/>
-    <col min="8" max="8" width="17.5546875" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="12.77734375" style="35"/>
+    <col min="5" max="5" width="13.6328125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="35"/>
+    <col min="8" max="8" width="17.54296875" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -17671,7 +17671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
@@ -17697,7 +17697,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C3" s="52" t="s">
         <v>269</v>
       </c>
@@ -17717,7 +17717,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C4" s="52" t="s">
         <v>270</v>
       </c>
@@ -17737,7 +17737,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>58</v>
       </c>
@@ -17763,7 +17763,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C6" s="52" t="s">
         <v>270</v>
       </c>
@@ -17783,7 +17783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>65</v>
       </c>
@@ -17806,7 +17806,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C8" s="52" t="s">
         <v>270</v>
       </c>
@@ -17826,7 +17826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>136</v>
       </c>
@@ -17852,7 +17852,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C10" s="52" t="s">
         <v>270</v>
       </c>
@@ -17872,7 +17872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
         <v>65</v>
       </c>
@@ -17895,7 +17895,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
         <v>270</v>
       </c>
@@ -17915,7 +17915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>61</v>
       </c>
@@ -17941,7 +17941,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C14" s="52" t="s">
         <v>270</v>
       </c>
@@ -17962,7 +17962,7 @@
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
         <v>65</v>
       </c>
@@ -17986,7 +17986,7 @@
       </c>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
         <v>270</v>
       </c>
@@ -18007,7 +18007,7 @@
       </c>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>62</v>
       </c>
@@ -18034,7 +18034,7 @@
       </c>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
         <v>269</v>
       </c>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>63</v>
       </c>
@@ -18081,7 +18081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C20" s="52" t="s">
         <v>269</v>
       </c>
@@ -18101,7 +18101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>64</v>
       </c>
@@ -18127,7 +18127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C22" s="52" t="s">
         <v>269</v>
       </c>
@@ -18147,7 +18147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>79</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C24" s="52" t="s">
         <v>269</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C25" s="52" t="s">
         <v>270</v>
       </c>
@@ -18213,7 +18213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>80</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C27" s="52" t="s">
         <v>269</v>
       </c>
@@ -18259,7 +18259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C28" s="52" t="s">
         <v>270</v>
       </c>
@@ -18279,7 +18279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>81</v>
       </c>
@@ -18305,7 +18305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C30" s="52" t="s">
         <v>269</v>
       </c>
@@ -18325,7 +18325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C31" s="52" t="s">
         <v>270</v>
       </c>
@@ -18345,7 +18345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>82</v>
       </c>
@@ -18371,7 +18371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C33" s="52" t="s">
         <v>269</v>
       </c>
@@ -18391,7 +18391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C34" s="52" t="s">
         <v>270</v>
       </c>
@@ -18411,7 +18411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>83</v>
       </c>
@@ -18437,7 +18437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C36" s="52" t="s">
         <v>269</v>
       </c>
@@ -18457,7 +18457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C37" s="52" t="s">
         <v>270</v>
       </c>
@@ -18477,7 +18477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>60</v>
       </c>
@@ -18503,7 +18503,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C39" s="52" t="s">
         <v>269</v>
       </c>
@@ -18523,7 +18523,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C40" s="52" t="s">
         <v>270</v>
       </c>
@@ -18543,7 +18543,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B41" s="52" t="s">
         <v>16</v>
       </c>
@@ -18566,7 +18566,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C42" s="52" t="s">
         <v>269</v>
       </c>
@@ -18586,7 +18586,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C43" s="52" t="s">
         <v>270</v>
       </c>
@@ -18606,7 +18606,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
         <v>84</v>
       </c>
@@ -18632,7 +18632,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C45" s="52" t="s">
         <v>269</v>
       </c>
@@ -18652,7 +18652,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
         <v>85</v>
       </c>
@@ -18678,7 +18678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C47" s="52" t="s">
         <v>269</v>
       </c>
@@ -18698,7 +18698,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
         <v>196</v>
       </c>
@@ -18724,7 +18724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C49" s="52" t="s">
         <v>269</v>
       </c>
@@ -18762,16 +18762,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="35" customWidth="1"/>
-    <col min="4" max="7" width="17.21875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.77734375" style="35"/>
+    <col min="2" max="2" width="27.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" style="35" customWidth="1"/>
+    <col min="4" max="7" width="17.1796875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.81640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="132" t="s">
         <v>69</v>
       </c>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="H1" s="103"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>86</v>
       </c>
@@ -18817,7 +18817,7 @@
       </c>
       <c r="H2" s="97"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C3" s="35" t="s">
         <v>269</v>
       </c>
@@ -18835,7 +18835,7 @@
       </c>
       <c r="H3" s="141"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>87</v>
       </c>
@@ -18859,7 +18859,7 @@
       </c>
       <c r="H4" s="141"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="C5" s="35" t="s">
         <v>269</v>
@@ -18878,7 +18878,7 @@
       </c>
       <c r="H5" s="97"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>88</v>
       </c>
@@ -18902,7 +18902,7 @@
       </c>
       <c r="H6" s="97"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="C7" s="35" t="s">
         <v>269</v>
@@ -18938,14 +18938,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -18956,7 +18956,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -19055,7 +19055,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -19261,7 +19261,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -19377,13 +19377,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -19804,13 +19804,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
-    <col min="2" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -19940,13 +19940,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -19981,7 +19981,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -19998,10 +19998,10 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -20018,10 +20018,10 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -20038,7 +20038,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
@@ -20052,7 +20052,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
@@ -20066,7 +20066,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -20083,7 +20083,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
@@ -20097,7 +20097,7 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
@@ -20114,7 +20114,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
@@ -20145,15 +20145,15 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="35" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="35"/>
+    <col min="2" max="2" width="19.08984375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>178</v>
       </c>
@@ -20170,7 +20170,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>173</v>
       </c>
@@ -20184,7 +20184,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="46" t="s">
         <v>1</v>
@@ -20198,7 +20198,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="46" t="s">
         <v>2</v>
@@ -20212,7 +20212,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="46" t="s">
         <v>3</v>
@@ -20226,7 +20226,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="46" t="s">
         <v>4</v>
@@ -20240,7 +20240,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="46" t="s">
         <v>172</v>
@@ -20249,7 +20249,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="84"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
         <v>199</v>
       </c>
@@ -20265,7 +20265,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="46" t="s">
         <v>1</v>
@@ -20277,7 +20277,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="46" t="s">
         <v>2</v>
@@ -20289,7 +20289,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="46" t="s">
         <v>3</v>
@@ -20301,7 +20301,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="46" t="s">
         <v>4</v>
@@ -20313,7 +20313,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="46" t="s">
         <v>172</v>
@@ -20322,7 +20322,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="84"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
         <v>200</v>
       </c>
@@ -20338,7 +20338,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="46" t="s">
         <v>1</v>
@@ -20352,7 +20352,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="46" t="s">
         <v>2</v>
@@ -20366,7 +20366,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="46" t="s">
         <v>3</v>
@@ -20380,7 +20380,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="46" t="s">
         <v>4</v>
@@ -20394,7 +20394,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="46" t="s">
         <v>172</v>
@@ -20421,15 +20421,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
         <v>164</v>
       </c>
@@ -20443,7 +20443,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>69</v>
       </c>
@@ -20455,7 +20455,7 @@
       </c>
       <c r="D2" s="84"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="65" t="s">
         <v>185</v>
       </c>
@@ -20480,21 +20480,21 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="52" customWidth="1"/>
     <col min="2" max="2" width="20" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.44140625" style="35"/>
+    <col min="3" max="3" width="20.453125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="32.36328125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.453125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>69</v>
       </c>
@@ -20784,7 +20784,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>173</v>
       </c>
@@ -20795,7 +20795,7 @@
         <v>0.95</v>
       </c>
       <c r="D18" s="87">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;"")*('IYCF packages'!$C$2:$E$6&lt;&gt;FALSE))</f>
         <v>3.66</v>
       </c>
       <c r="E18" s="86" t="s">
@@ -20813,8 +20813,8 @@
         <v>0.95</v>
       </c>
       <c r="D19" s="87">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
-        <v>3.78</v>
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;"")*('IYCF packages'!$C$9:$E$13&lt;&gt;FALSE))</f>
+        <v>0</v>
       </c>
       <c r="E19" s="86" t="s">
         <v>202</v>
@@ -20831,7 +20831,7 @@
         <v>0.95</v>
       </c>
       <c r="D20" s="87">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;"")*('IYCF packages'!$C$16:$E$20&lt;&gt;FALSE))</f>
         <v>14.270000000000001</v>
       </c>
       <c r="E20" s="86" t="s">

</xml_diff>

<commit_message>
And also for demo multi-region
</commit_message>
<xml_diff>
--- a/inputs/demo_region2_input.xlsx
+++ b/inputs/demo_region2_input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\applications\demo\data\regional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21144" windowWidth="38400" windowHeight="21144" tabRatio="961" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="-38400" yWindow="-21144" windowWidth="38400" windowHeight="21144" tabRatio="961" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -5757,7 +5757,7 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="C29" activeCellId="3" sqref="C2:O12 C14:O21 C23:O27 C29:O38"/>
     </sheetView>
   </sheetViews>
@@ -12814,12 +12814,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12829,6 +12823,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -20141,8 +20141,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20257,9 +20257,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="84"/>
-      <c r="D9" s="84" t="b">
-        <v>0</v>
-      </c>
+      <c r="D9" s="84"/>
       <c r="E9" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20271,7 +20269,9 @@
         <v>1</v>
       </c>
       <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="D10" s="84" t="s">
+        <v>194</v>
+      </c>
       <c r="E10" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20283,7 +20283,9 @@
         <v>2</v>
       </c>
       <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
+      <c r="D11" s="84" t="s">
+        <v>194</v>
+      </c>
       <c r="E11" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20295,7 +20297,9 @@
         <v>3</v>
       </c>
       <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
+      <c r="D12" s="84" t="s">
+        <v>194</v>
+      </c>
       <c r="E12" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20307,7 +20311,9 @@
         <v>4</v>
       </c>
       <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
+      <c r="D13" s="84" t="s">
+        <v>194</v>
+      </c>
       <c r="E13" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20329,10 +20335,10 @@
       <c r="B16" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84" t="s">
+      <c r="C16" s="84" t="s">
         <v>194</v>
       </c>
+      <c r="D16" s="84"/>
       <c r="E16" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20344,9 +20350,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="84"/>
-      <c r="D17" s="84" t="s">
-        <v>194</v>
-      </c>
+      <c r="D17" s="84"/>
       <c r="E17" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20358,9 +20362,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="84"/>
-      <c r="D18" s="84" t="s">
-        <v>194</v>
-      </c>
+      <c r="D18" s="84"/>
       <c r="E18" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20372,9 +20374,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="84"/>
-      <c r="D19" s="84" t="s">
-        <v>194</v>
-      </c>
+      <c r="D19" s="84"/>
       <c r="E19" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20386,9 +20386,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="84"/>
-      <c r="D20" s="84" t="s">
-        <v>194</v>
-      </c>
+      <c r="D20" s="84"/>
       <c r="E20" s="61" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -20814,7 +20812,7 @@
       </c>
       <c r="D19" s="87">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
-        <v>3.78</v>
+        <v>10.49</v>
       </c>
       <c r="E19" s="86" t="s">
         <v>202</v>
@@ -20832,7 +20830,7 @@
       </c>
       <c r="D20" s="87">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
-        <v>14.270000000000001</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="E20" s="86" t="s">
         <v>202</v>

</xml_diff>